<commit_message>
added graphing of the produced solution
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wing's stuff\TUD\yr 4\q1\Operations and Optimisations\group assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wing's stuff\TUD\yr 4\q1\Operations and Optimisations\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37805C35-4241-4BEE-A4F9-02F51AD3E083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A08D8E4-6DE8-44D1-B785-F021CF5DD819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="4872" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="something" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>From</t>
   </si>
@@ -463,9 +463,9 @@
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -498,7 +498,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -608,7 +608,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -619,7 +619,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -630,7 +630,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -663,7 +663,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -685,7 +685,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -714,15 +714,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F72362-0205-4B86-AEA5-584F42E1BE5B}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -756,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -773,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -790,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -804,6 +804,91 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>-4</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-2</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>-2</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-4</v>
+      </c>
+      <c r="C10">
+        <v>-2</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>